<commit_message>
All code done, maybe i will refactor later
</commit_message>
<xml_diff>
--- a/KMZI_Lab5/Grapics_Lab5.xlsx
+++ b/KMZI_Lab5/Grapics_Lab5.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\valda\source\repos\semester#6\КМЗИ\KMZI_Lab5\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AFD1F20-5EE2-4912-87A5-A67C2220536F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A29C8EF1-CE12-493A-8098-67DF43B68E47}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-104" yWindow="-104" windowWidth="22326" windowHeight="12200" xr2:uid="{8A69AB49-B81E-4E74-895C-A88182CF4507}"/>
   </bookViews>
@@ -16,21 +16,22 @@
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Лист1!$B$3:$B$38</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Лист1!$C$2</definedName>
-    <definedName name="_xlchart.v1.10" hidden="1">Лист1!$C$2</definedName>
-    <definedName name="_xlchart.v1.11" hidden="1">Лист1!$C$3:$C$36</definedName>
-    <definedName name="_xlchart.v1.12" hidden="1">Лист1!$B$3:$B$38</definedName>
-    <definedName name="_xlchart.v1.13" hidden="1">Лист1!$C$2</definedName>
-    <definedName name="_xlchart.v1.14" hidden="1">Лист1!$C$3:$C$38</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Лист1!$C$3:$C$38</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">Лист1!$B$3:$B$38</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">Лист1!$C$2</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">Лист1!$C$3:$C$38</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">Лист1!$E$3:$E$37</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">Лист1!$F$2</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">Лист1!$F$3:$F$37</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">Лист1!$B$3:$B$36</definedName>
+    <definedName name="_xlchart.v1.0" hidden="1">Лист1!$E$3:$E$37</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">Лист1!$F$2</definedName>
+    <definedName name="_xlchart.v1.10" hidden="1">Лист1!$I$2</definedName>
+    <definedName name="_xlchart.v1.11" hidden="1">Лист1!$I$3:$I$36</definedName>
+    <definedName name="_xlchart.v1.12" hidden="1">Лист1!$I$3:$I$37</definedName>
+    <definedName name="_xlchart.v1.13" hidden="1">Лист1!$B$3:$B$38</definedName>
+    <definedName name="_xlchart.v1.14" hidden="1">Лист1!$C$2</definedName>
+    <definedName name="_xlchart.v1.15" hidden="1">Лист1!$C$3:$C$38</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">Лист1!$F$3:$F$37</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">Лист1!$B$3:$B$37</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">Лист1!$B$3:$B$38</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">Лист1!$C$2</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">Лист1!$C$3:$C$37</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">Лист1!$C$3:$C$38</definedName>
+    <definedName name="_xlchart.v1.8" hidden="1">Лист1!$H$3:$H$36</definedName>
+    <definedName name="_xlchart.v1.9" hidden="1">Лист1!$H$3:$H$37</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -47,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="40">
   <si>
     <t>,</t>
   </si>
@@ -370,10 +371,10 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.6</cx:f>
+        <cx:f>_xlchart.v1.0</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.8</cx:f>
+        <cx:f>_xlchart.v1.2</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -381,7 +382,7 @@
     <cx:title pos="t" align="ctr" overlay="0">
       <cx:tx>
         <cx:txData>
-          <cx:v>Шифротекст (маршрутный шифр)</cx:v>
+          <cx:v>Шифротекст (маршрутная перестановка)</cx:v>
         </cx:txData>
       </cx:tx>
       <cx:txPr>
@@ -401,7 +402,7 @@
               </a:solidFill>
               <a:latin typeface="Calibri" panose="020F0502020204030204"/>
             </a:rPr>
-            <a:t>Шифротекст (маршрутный шифр)</a:t>
+            <a:t>Шифротекст (маршрутная перестановка)</a:t>
           </a:r>
         </a:p>
       </cx:txPr>
@@ -411,7 +412,7 @@
         <cx:series layoutId="clusteredColumn" uniqueId="{1950A1F1-94A4-441E-9448-693592FF9D8F}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.7</cx:f>
+              <cx:f>_xlchart.v1.1</cx:f>
               <cx:v>Appearances</cx:v>
             </cx:txData>
           </cx:tx>
@@ -469,10 +470,10 @@
   <cx:chartData>
     <cx:data id="0">
       <cx:strDim type="cat">
-        <cx:f>_xlchart.v1.0</cx:f>
+        <cx:f>_xlchart.v1.3</cx:f>
       </cx:strDim>
       <cx:numDim type="val">
-        <cx:f>_xlchart.v1.2</cx:f>
+        <cx:f>_xlchart.v1.6</cx:f>
       </cx:numDim>
     </cx:data>
   </cx:chartData>
@@ -510,7 +511,7 @@
         <cx:series layoutId="clusteredColumn" uniqueId="{1CC52DD7-ED4B-4387-8A99-1B623818A478}">
           <cx:tx>
             <cx:txData>
-              <cx:f>_xlchart.v1.1</cx:f>
+              <cx:f>_xlchart.v1.5</cx:f>
               <cx:v>Appearances</cx:v>
             </cx:txData>
           </cx:tx>
@@ -529,6 +530,106 @@
           <cx:axisId val="1"/>
         </cx:series>
         <cx:series layoutId="paretoLine" ownerIdx="0" uniqueId="{386BF15E-350D-4839-96AF-33CFA1240621}">
+          <cx:spPr>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </cx:spPr>
+          <cx:axisId val="2"/>
+        </cx:series>
+      </cx:plotAreaRegion>
+      <cx:axis id="0">
+        <cx:catScaling gapWidth="0"/>
+        <cx:tickLabels/>
+      </cx:axis>
+      <cx:axis id="1">
+        <cx:valScaling/>
+        <cx:majorGridlines/>
+        <cx:majorTickMarks type="in"/>
+        <cx:tickLabels/>
+      </cx:axis>
+      <cx:axis id="2" hidden="1">
+        <cx:valScaling max="1" min="0"/>
+        <cx:units unit="percentage"/>
+        <cx:tickLabels/>
+      </cx:axis>
+    </cx:plotArea>
+  </cx:chart>
+  <cx:spPr>
+    <a:ln>
+      <a:solidFill>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:solidFill>
+    </a:ln>
+  </cx:spPr>
+</cx:chartSpace>
+</file>
+
+<file path=xl/charts/chartEx3.xml><?xml version="1.0" encoding="utf-8"?>
+<cx:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex">
+  <cx:chartData>
+    <cx:data id="0">
+      <cx:strDim type="cat">
+        <cx:f>_xlchart.v1.9</cx:f>
+      </cx:strDim>
+      <cx:numDim type="val">
+        <cx:f>_xlchart.v1.12</cx:f>
+      </cx:numDim>
+    </cx:data>
+  </cx:chartData>
+  <cx:chart>
+    <cx:title pos="t" align="ctr" overlay="0">
+      <cx:tx>
+        <cx:txData>
+          <cx:v>Шифротекст (множественная перестановка)</cx:v>
+        </cx:txData>
+      </cx:tx>
+      <cx:txPr>
+        <a:bodyPr spcFirstLastPara="1" vertOverflow="ellipsis" horzOverflow="overflow" wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr" rtl="0">
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="ru-RU" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+              <a:solidFill>
+                <a:sysClr val="windowText" lastClr="000000">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:sysClr>
+              </a:solidFill>
+              <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+            </a:rPr>
+            <a:t>Шифротекст (множественная перестановка)</a:t>
+          </a:r>
+        </a:p>
+      </cx:txPr>
+    </cx:title>
+    <cx:plotArea>
+      <cx:plotAreaRegion>
+        <cx:series layoutId="clusteredColumn" uniqueId="{D389253E-C393-48A1-A1DE-72048F1C754C}">
+          <cx:tx>
+            <cx:txData>
+              <cx:f>_xlchart.v1.10</cx:f>
+              <cx:v>Appearances</cx:v>
+            </cx:txData>
+          </cx:tx>
+          <cx:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2">
+                <a:lumMod val="40000"/>
+                <a:lumOff val="60000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </cx:spPr>
+          <cx:dataId val="0"/>
+          <cx:layoutPr>
+            <cx:aggregation/>
+          </cx:layoutPr>
+          <cx:axisId val="1"/>
+        </cx:series>
+        <cx:series layoutId="paretoLine" ownerIdx="0" uniqueId="{F3F3ABA5-4F53-4DE4-82C6-CBF5FFAD9B7B}">
           <cx:spPr>
             <a:ln>
               <a:noFill/>
@@ -643,6 +744,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="366">
   <cs:axisTitle>
@@ -1152,6 +1293,514 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="366">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat">
+        <a:solidFill>
+          <a:srgbClr val="D9D9D9"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="366">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -1665,14 +2314,14 @@
     <xdr:from>
       <xdr:col>11</xdr:col>
       <xdr:colOff>11832</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>168891</xdr:rowOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>5375</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>21</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>20</xdr:row>
-      <xdr:rowOff>154909</xdr:rowOff>
+      <xdr:rowOff>172121</xdr:rowOff>
     </xdr:to>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
@@ -1708,7 +2357,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="7628246" y="2088056"/>
+              <a:off x="7886430" y="2105268"/>
               <a:ext cx="6442756" cy="1793302"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -1786,8 +2435,86 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="7615339" y="297987"/>
+              <a:off x="7873523" y="297987"/>
               <a:ext cx="6464270" cy="1612571"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:solidFill>
+              <a:prstClr val="white"/>
+            </a:solidFill>
+            <a:ln w="1">
+              <a:solidFill>
+                <a:prstClr val="green"/>
+              </a:solidFill>
+            </a:ln>
+          </xdr:spPr>
+          <xdr:txBody>
+            <a:bodyPr vertOverflow="clip" horzOverflow="clip"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:r>
+                <a:rPr lang="ru-BY" sz="1100"/>
+                <a:t>Эта диаграмма недоступна в вашей версии Excel.
+Изменение этой фигуры или сохранение книги в другом формате приведет к остаточному повреждению диаграммы.</a:t>
+              </a:r>
+            </a:p>
+          </xdr:txBody>
+        </xdr:sp>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>645458</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>3031</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>17212</xdr:rowOff>
+    </xdr:to>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" Requires="cx1">
+        <xdr:graphicFrame macro="">
+          <xdr:nvGraphicFramePr>
+            <xdr:cNvPr id="2" name="Диаграмма 1">
+              <a:extLst>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{20F949FE-F9AC-4125-87FC-9522260C524E}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvGraphicFramePr/>
+          </xdr:nvGraphicFramePr>
+          <xdr:xfrm>
+            <a:off x="0" y="0"/>
+            <a:ext cx="0" cy="0"/>
+          </xdr:xfrm>
+          <a:graphic>
+            <a:graphicData uri="http://schemas.microsoft.com/office/drawing/2014/chartex">
+              <cx:chart xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+            </a:graphicData>
+          </a:graphic>
+        </xdr:graphicFrame>
+      </mc:Choice>
+      <mc:Fallback>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="0" name=""/>
+            <xdr:cNvSpPr>
+              <a:spLocks noTextEdit="1"/>
+            </xdr:cNvSpPr>
+          </xdr:nvSpPr>
+          <xdr:spPr>
+            <a:xfrm>
+              <a:off x="7874597" y="4090937"/>
+              <a:ext cx="6454589" cy="1821466"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
               <a:avLst/>
@@ -2119,8 +2846,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{02556EC1-531B-4B1F-81CC-000C9BEFF3E2}">
   <dimension ref="B1:I37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+    <sheetView tabSelected="1" topLeftCell="B10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="K31" sqref="K31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2133,7 +2860,7 @@
     <col min="9" max="9" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" ht="23.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:9" ht="19.05" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B1" s="4" t="s">
         <v>36</v>
       </c>
@@ -2180,6 +2907,12 @@
       <c r="F3" s="2">
         <v>240</v>
       </c>
+      <c r="H3" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="I3" s="2">
+        <v>240</v>
+      </c>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B4" s="2" t="s">
@@ -2194,6 +2927,12 @@
       <c r="F4" s="2">
         <v>204</v>
       </c>
+      <c r="H4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I4" s="2">
+        <v>118</v>
+      </c>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B5" s="2" t="s">
@@ -2208,6 +2947,12 @@
       <c r="F5" s="2">
         <v>198</v>
       </c>
+      <c r="H5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I5" s="2">
+        <v>177</v>
+      </c>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B6" s="2" t="s">
@@ -2222,6 +2967,12 @@
       <c r="F6" s="2">
         <v>78</v>
       </c>
+      <c r="H6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I6" s="2">
+        <v>575</v>
+      </c>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B7" s="2" t="s">
@@ -2236,6 +2987,12 @@
       <c r="F7" s="2">
         <v>575</v>
       </c>
+      <c r="H7" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I7" s="2">
+        <v>334</v>
+      </c>
     </row>
     <row r="8" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B8" s="2" t="s">
@@ -2250,6 +3007,12 @@
       <c r="F8" s="2">
         <v>154</v>
       </c>
+      <c r="H8" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="I8" s="2">
+        <v>20</v>
+      </c>
     </row>
     <row r="9" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B9" s="2" t="s">
@@ -2264,6 +3027,12 @@
       <c r="F9" s="2">
         <v>73</v>
       </c>
+      <c r="H9" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="I9" s="2">
+        <v>133</v>
+      </c>
     </row>
     <row r="10" spans="2:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="2" t="s">
@@ -2278,6 +3047,12 @@
       <c r="F10" s="2">
         <v>85</v>
       </c>
+      <c r="H10" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I10" s="2">
+        <v>675</v>
+      </c>
     </row>
     <row r="11" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B11" s="2" t="s">
@@ -2292,6 +3067,12 @@
       <c r="F11" s="2">
         <v>184</v>
       </c>
+      <c r="H11" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I11" s="2">
+        <v>184</v>
+      </c>
     </row>
     <row r="12" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B12" s="2" t="s">
@@ -2306,6 +3087,12 @@
       <c r="F12" s="2">
         <v>675</v>
       </c>
+      <c r="H12" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="I12" s="2">
+        <v>148</v>
+      </c>
     </row>
     <row r="13" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B13" s="2" t="s">
@@ -2320,6 +3107,12 @@
       <c r="F13" s="2">
         <v>88</v>
       </c>
+      <c r="H13" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I13" s="2">
+        <v>48</v>
+      </c>
     </row>
     <row r="14" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B14" s="2" t="s">
@@ -2334,6 +3127,12 @@
       <c r="F14" s="2">
         <v>337</v>
       </c>
+      <c r="H14" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I14" s="2">
+        <v>204</v>
+      </c>
     </row>
     <row r="15" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B15" s="2" t="s">
@@ -2348,6 +3147,12 @@
       <c r="F15" s="2">
         <v>5</v>
       </c>
+      <c r="H15" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I15" s="2">
+        <v>41</v>
+      </c>
     </row>
     <row r="16" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B16" s="2" t="s">
@@ -2362,8 +3167,14 @@
       <c r="F16" s="2">
         <v>133</v>
       </c>
+      <c r="H16" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I16" s="2">
+        <v>198</v>
+      </c>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B17" s="2" t="s">
         <v>21</v>
       </c>
@@ -2376,8 +3187,14 @@
       <c r="F17" s="2">
         <v>334</v>
       </c>
+      <c r="H17" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="I17" s="2">
+        <v>88</v>
+      </c>
     </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B18" s="2" t="s">
         <v>22</v>
       </c>
@@ -2390,8 +3207,14 @@
       <c r="F18" s="2">
         <v>188</v>
       </c>
+      <c r="H18" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="I18" s="2">
+        <v>188</v>
+      </c>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B19" s="2" t="s">
         <v>23</v>
       </c>
@@ -2404,8 +3227,14 @@
       <c r="F19" s="2">
         <v>148</v>
       </c>
+      <c r="H19" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="I19" s="2">
+        <v>6</v>
+      </c>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B20" s="2" t="s">
         <v>24</v>
       </c>
@@ -2418,8 +3247,14 @@
       <c r="F20" s="2">
         <v>177</v>
       </c>
+      <c r="H20" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="I20" s="2">
+        <v>16</v>
+      </c>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B21" s="2" t="s">
         <v>25</v>
       </c>
@@ -2432,8 +3267,14 @@
       <c r="F21" s="2">
         <v>48</v>
       </c>
+      <c r="H21" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I21" s="2">
+        <v>78</v>
+      </c>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B22" s="2" t="s">
         <v>26</v>
       </c>
@@ -2446,8 +3287,14 @@
       <c r="F22" s="2">
         <v>20</v>
       </c>
+      <c r="H22" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="I22" s="2">
+        <v>14</v>
+      </c>
     </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B23" s="2" t="s">
         <v>27</v>
       </c>
@@ -2460,8 +3307,14 @@
       <c r="F23" s="2">
         <v>34</v>
       </c>
+      <c r="H23" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="I23" s="2">
+        <v>337</v>
+      </c>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B24" s="2" t="s">
         <v>28</v>
       </c>
@@ -2474,8 +3327,14 @@
       <c r="F24" s="2">
         <v>16</v>
       </c>
+      <c r="H24" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="I24" s="2">
+        <v>85</v>
+      </c>
     </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B25" s="2" t="s">
         <v>29</v>
       </c>
@@ -2488,8 +3347,14 @@
       <c r="F25" s="2">
         <v>15</v>
       </c>
+      <c r="H25" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="I25" s="2">
+        <v>73</v>
+      </c>
     </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B26" s="2" t="s">
         <v>30</v>
       </c>
@@ -2502,8 +3367,14 @@
       <c r="F26" s="2">
         <v>118</v>
       </c>
+      <c r="H26" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="I26" s="2">
+        <v>34</v>
+      </c>
     </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B27" s="2" t="s">
         <v>31</v>
       </c>
@@ -2516,8 +3387,14 @@
       <c r="F27" s="2">
         <v>33</v>
       </c>
+      <c r="H27" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="I27" s="2">
+        <v>154</v>
+      </c>
     </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B28" s="2" t="s">
         <v>32</v>
       </c>
@@ -2530,8 +3407,14 @@
       <c r="F28" s="2">
         <v>41</v>
       </c>
+      <c r="H28" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="I28" s="2">
+        <v>7</v>
+      </c>
     </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B29" s="2" t="s">
         <v>33</v>
       </c>
@@ -2544,8 +3427,14 @@
       <c r="F29" s="2">
         <v>68</v>
       </c>
+      <c r="H29" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="I29" s="2">
+        <v>68</v>
+      </c>
     </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B30" s="2" t="s">
         <v>3</v>
       </c>
@@ -2558,8 +3447,14 @@
       <c r="F30" s="2">
         <v>12</v>
       </c>
+      <c r="H30" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="I30" s="2">
+        <v>5</v>
+      </c>
     </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B31" s="2" t="s">
         <v>5</v>
       </c>
@@ -2572,8 +3467,14 @@
       <c r="F31" s="2">
         <v>11</v>
       </c>
+      <c r="H31" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="I31" s="2">
+        <v>2</v>
+      </c>
     </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B32" s="2" t="s">
         <v>12</v>
       </c>
@@ -2586,8 +3487,14 @@
       <c r="F32" s="2">
         <v>6</v>
       </c>
+      <c r="H32" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="I32" s="2">
+        <v>3</v>
+      </c>
     </row>
-    <row r="33" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B33" s="3" t="s">
         <v>6</v>
       </c>
@@ -2600,8 +3507,14 @@
       <c r="F33" s="2">
         <v>7</v>
       </c>
+      <c r="H33" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="I33" s="2">
+        <v>15</v>
+      </c>
     </row>
-    <row r="34" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B34" s="2" t="s">
         <v>4</v>
       </c>
@@ -2614,8 +3527,14 @@
       <c r="F34" s="2">
         <v>2</v>
       </c>
+      <c r="H34" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="I34" s="2">
+        <v>11</v>
+      </c>
     </row>
-    <row r="35" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B35" s="2" t="s">
         <v>1</v>
       </c>
@@ -2628,8 +3547,14 @@
       <c r="F35" s="2">
         <v>14</v>
       </c>
+      <c r="H35" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="I35" s="2">
+        <v>1</v>
+      </c>
     </row>
-    <row r="36" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B36" s="2" t="s">
         <v>2</v>
       </c>
@@ -2642,8 +3567,14 @@
       <c r="F36" s="2">
         <v>3</v>
       </c>
+      <c r="H36" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="I36" s="2">
+        <v>12</v>
+      </c>
     </row>
-    <row r="37" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:9" x14ac:dyDescent="0.3">
       <c r="B37" s="2" t="s">
         <v>0</v>
       </c>
@@ -2655,6 +3586,12 @@
       </c>
       <c r="F37" s="2">
         <v>1</v>
+      </c>
+      <c r="H37" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="I37" s="2">
+        <v>33</v>
       </c>
     </row>
   </sheetData>

</xml_diff>